<commit_message>
Add File Function MyMoney
</commit_message>
<xml_diff>
--- a/Description of FinanceManagement Softwares.xlsx
+++ b/Description of FinanceManagement Softwares.xlsx
@@ -865,7 +865,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -944,53 +944,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1010,6 +965,54 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1314,7 +1317,7 @@
   <dimension ref="B1:D119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1328,11 +1331,11 @@
   <sheetData>
     <row r="1" spans="2:4" ht="6.75" customHeight="1"/>
     <row r="2" spans="2:4">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="36"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="46"/>
     </row>
     <row r="3" spans="2:4">
       <c r="B3" s="8" t="s">
@@ -1346,7 +1349,7 @@
       </c>
     </row>
     <row r="4" spans="2:4">
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="47" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -1357,16 +1360,16 @@
       </c>
     </row>
     <row r="5" spans="2:4">
-      <c r="B5" s="38"/>
+      <c r="B5" s="48"/>
       <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="28" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="2:4">
-      <c r="B6" s="39"/>
+      <c r="B6" s="49"/>
       <c r="C6" s="7" t="s">
         <v>7</v>
       </c>
@@ -1375,7 +1378,7 @@
       </c>
     </row>
     <row r="7" spans="2:4">
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="47" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -1386,7 +1389,7 @@
       </c>
     </row>
     <row r="8" spans="2:4">
-      <c r="B8" s="38"/>
+      <c r="B8" s="48"/>
       <c r="C8" s="5" t="s">
         <v>10</v>
       </c>
@@ -1395,14 +1398,14 @@
       </c>
     </row>
     <row r="9" spans="2:4">
-      <c r="B9" s="39"/>
+      <c r="B9" s="49"/>
       <c r="C9" s="7" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="7"/>
     </row>
     <row r="10" spans="2:4">
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="47" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -1413,7 +1416,7 @@
       </c>
     </row>
     <row r="11" spans="2:4">
-      <c r="B11" s="38"/>
+      <c r="B11" s="48"/>
       <c r="C11" s="5" t="s">
         <v>18</v>
       </c>
@@ -1422,7 +1425,7 @@
       </c>
     </row>
     <row r="12" spans="2:4">
-      <c r="B12" s="38"/>
+      <c r="B12" s="48"/>
       <c r="C12" s="5" t="s">
         <v>20</v>
       </c>
@@ -1431,7 +1434,7 @@
       </c>
     </row>
     <row r="13" spans="2:4">
-      <c r="B13" s="38"/>
+      <c r="B13" s="48"/>
       <c r="C13" s="5" t="s">
         <v>21</v>
       </c>
@@ -1440,7 +1443,7 @@
       </c>
     </row>
     <row r="14" spans="2:4">
-      <c r="B14" s="38"/>
+      <c r="B14" s="48"/>
       <c r="C14" s="5" t="s">
         <v>22</v>
       </c>
@@ -1449,7 +1452,7 @@
       </c>
     </row>
     <row r="15" spans="2:4">
-      <c r="B15" s="39"/>
+      <c r="B15" s="49"/>
       <c r="C15" s="7" t="s">
         <v>23</v>
       </c>
@@ -1467,7 +1470,7 @@
       </c>
     </row>
     <row r="17" spans="2:4">
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="47" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -1478,7 +1481,7 @@
       </c>
     </row>
     <row r="18" spans="2:4">
-      <c r="B18" s="38"/>
+      <c r="B18" s="48"/>
       <c r="C18" s="5" t="s">
         <v>28</v>
       </c>
@@ -1487,7 +1490,7 @@
       </c>
     </row>
     <row r="19" spans="2:4">
-      <c r="B19" s="39"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="7" t="s">
         <v>29</v>
       </c>
@@ -1496,7 +1499,7 @@
       </c>
     </row>
     <row r="20" spans="2:4">
-      <c r="B20" s="37" t="s">
+      <c r="B20" s="47" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -1507,7 +1510,7 @@
       </c>
     </row>
     <row r="21" spans="2:4">
-      <c r="B21" s="38"/>
+      <c r="B21" s="48"/>
       <c r="C21" s="5" t="s">
         <v>33</v>
       </c>
@@ -1516,7 +1519,7 @@
       </c>
     </row>
     <row r="22" spans="2:4">
-      <c r="B22" s="38"/>
+      <c r="B22" s="48"/>
       <c r="C22" s="5" t="s">
         <v>35</v>
       </c>
@@ -1525,7 +1528,7 @@
       </c>
     </row>
     <row r="23" spans="2:4">
-      <c r="B23" s="38"/>
+      <c r="B23" s="48"/>
       <c r="C23" s="5" t="s">
         <v>37</v>
       </c>
@@ -1534,7 +1537,7 @@
       </c>
     </row>
     <row r="24" spans="2:4">
-      <c r="B24" s="39"/>
+      <c r="B24" s="49"/>
       <c r="C24" s="7" t="s">
         <v>39</v>
       </c>
@@ -1552,7 +1555,7 @@
       </c>
     </row>
     <row r="26" spans="2:4">
-      <c r="B26" s="37" t="s">
+      <c r="B26" s="47" t="s">
         <v>42</v>
       </c>
       <c r="C26" s="4" t="s">
@@ -1563,7 +1566,7 @@
       </c>
     </row>
     <row r="27" spans="2:4">
-      <c r="B27" s="38"/>
+      <c r="B27" s="48"/>
       <c r="C27" s="5" t="s">
         <v>44</v>
       </c>
@@ -1572,7 +1575,7 @@
       </c>
     </row>
     <row r="28" spans="2:4">
-      <c r="B28" s="38"/>
+      <c r="B28" s="48"/>
       <c r="C28" s="5" t="s">
         <v>45</v>
       </c>
@@ -1581,7 +1584,7 @@
       </c>
     </row>
     <row r="29" spans="2:4">
-      <c r="B29" s="38"/>
+      <c r="B29" s="48"/>
       <c r="C29" s="5" t="s">
         <v>46</v>
       </c>
@@ -1590,7 +1593,7 @@
       </c>
     </row>
     <row r="30" spans="2:4">
-      <c r="B30" s="38"/>
+      <c r="B30" s="48"/>
       <c r="C30" s="5" t="s">
         <v>48</v>
       </c>
@@ -1599,7 +1602,7 @@
       </c>
     </row>
     <row r="31" spans="2:4">
-      <c r="B31" s="39"/>
+      <c r="B31" s="49"/>
       <c r="C31" s="7" t="s">
         <v>50</v>
       </c>
@@ -1631,11 +1634,11 @@
       <c r="D34" s="2"/>
     </row>
     <row r="35" spans="2:4">
-      <c r="B35" s="40" t="s">
+      <c r="B35" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="C35" s="41"/>
-      <c r="D35" s="42"/>
+      <c r="C35" s="51"/>
+      <c r="D35" s="52"/>
     </row>
     <row r="36" spans="2:4">
       <c r="B36" s="15" t="s">
@@ -1649,7 +1652,7 @@
       </c>
     </row>
     <row r="37" spans="2:4">
-      <c r="B37" s="31" t="s">
+      <c r="B37" s="40" t="s">
         <v>63</v>
       </c>
       <c r="C37" s="18" t="s">
@@ -1660,7 +1663,7 @@
       </c>
     </row>
     <row r="38" spans="2:4">
-      <c r="B38" s="32"/>
+      <c r="B38" s="41"/>
       <c r="C38" s="12" t="s">
         <v>66</v>
       </c>
@@ -1669,14 +1672,14 @@
       </c>
     </row>
     <row r="39" spans="2:4">
-      <c r="B39" s="32"/>
+      <c r="B39" s="41"/>
       <c r="C39" s="12" t="s">
         <v>68</v>
       </c>
       <c r="D39" s="12"/>
     </row>
     <row r="40" spans="2:4" ht="30">
-      <c r="B40" s="33"/>
+      <c r="B40" s="42"/>
       <c r="C40" s="14" t="s">
         <v>69</v>
       </c>
@@ -1685,7 +1688,7 @@
       </c>
     </row>
     <row r="41" spans="2:4" ht="30">
-      <c r="B41" s="31" t="s">
+      <c r="B41" s="40" t="s">
         <v>71</v>
       </c>
       <c r="C41" s="18" t="s">
@@ -1696,7 +1699,7 @@
       </c>
     </row>
     <row r="42" spans="2:4" ht="30">
-      <c r="B42" s="32"/>
+      <c r="B42" s="41"/>
       <c r="C42" s="12" t="s">
         <v>74</v>
       </c>
@@ -1705,7 +1708,7 @@
       </c>
     </row>
     <row r="43" spans="2:4">
-      <c r="B43" s="32"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="12" t="s">
         <v>79</v>
       </c>
@@ -1714,7 +1717,7 @@
       </c>
     </row>
     <row r="44" spans="2:4">
-      <c r="B44" s="33"/>
+      <c r="B44" s="42"/>
       <c r="C44" s="14" t="s">
         <v>76</v>
       </c>
@@ -1723,7 +1726,7 @@
       </c>
     </row>
     <row r="45" spans="2:4">
-      <c r="B45" s="31" t="s">
+      <c r="B45" s="40" t="s">
         <v>27</v>
       </c>
       <c r="C45" s="18" t="s">
@@ -1734,7 +1737,7 @@
       </c>
     </row>
     <row r="46" spans="2:4" ht="30">
-      <c r="B46" s="32"/>
+      <c r="B46" s="41"/>
       <c r="C46" s="12" t="s">
         <v>62</v>
       </c>
@@ -1743,7 +1746,7 @@
       </c>
     </row>
     <row r="47" spans="2:4">
-      <c r="B47" s="33"/>
+      <c r="B47" s="42"/>
       <c r="C47" s="14" t="s">
         <v>86</v>
       </c>
@@ -1752,7 +1755,7 @@
       </c>
     </row>
     <row r="48" spans="2:4">
-      <c r="B48" s="31" t="s">
+      <c r="B48" s="40" t="s">
         <v>80</v>
       </c>
       <c r="C48" s="18" t="s">
@@ -1763,7 +1766,7 @@
       </c>
     </row>
     <row r="49" spans="2:4">
-      <c r="B49" s="32"/>
+      <c r="B49" s="41"/>
       <c r="C49" s="12" t="s">
         <v>83</v>
       </c>
@@ -1772,7 +1775,7 @@
       </c>
     </row>
     <row r="50" spans="2:4">
-      <c r="B50" s="33"/>
+      <c r="B50" s="42"/>
       <c r="C50" s="14" t="s">
         <v>89</v>
       </c>
@@ -1781,7 +1784,7 @@
       </c>
     </row>
     <row r="51" spans="2:4">
-      <c r="B51" s="32" t="s">
+      <c r="B51" s="41" t="s">
         <v>87</v>
       </c>
       <c r="C51" s="12" t="s">
@@ -1792,7 +1795,7 @@
       </c>
     </row>
     <row r="52" spans="2:4" ht="30">
-      <c r="B52" s="32"/>
+      <c r="B52" s="41"/>
       <c r="C52" s="12" t="s">
         <v>91</v>
       </c>
@@ -1801,7 +1804,7 @@
       </c>
     </row>
     <row r="53" spans="2:4">
-      <c r="B53" s="33"/>
+      <c r="B53" s="42"/>
       <c r="C53" s="14" t="s">
         <v>95</v>
       </c>
@@ -1810,11 +1813,11 @@
       </c>
     </row>
     <row r="55" spans="2:4">
-      <c r="B55" s="28" t="s">
+      <c r="B55" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="C55" s="29"/>
-      <c r="D55" s="30"/>
+      <c r="C55" s="38"/>
+      <c r="D55" s="39"/>
     </row>
     <row r="56" spans="2:4">
       <c r="B56" s="15" t="s">
@@ -1828,14 +1831,14 @@
       </c>
     </row>
     <row r="57" spans="2:4">
-      <c r="B57" s="31" t="s">
+      <c r="B57" s="40" t="s">
         <v>98</v>
       </c>
       <c r="C57" s="25"/>
       <c r="D57" s="25"/>
     </row>
     <row r="58" spans="2:4">
-      <c r="B58" s="33"/>
+      <c r="B58" s="42"/>
       <c r="C58" s="23" t="s">
         <v>99</v>
       </c>
@@ -1844,14 +1847,14 @@
       </c>
     </row>
     <row r="59" spans="2:4">
-      <c r="B59" s="31" t="s">
+      <c r="B59" s="40" t="s">
         <v>101</v>
       </c>
       <c r="C59" s="25"/>
       <c r="D59" s="24"/>
     </row>
     <row r="60" spans="2:4">
-      <c r="B60" s="32"/>
+      <c r="B60" s="41"/>
       <c r="C60" s="26" t="s">
         <v>102</v>
       </c>
@@ -1860,7 +1863,7 @@
       </c>
     </row>
     <row r="61" spans="2:4">
-      <c r="B61" s="32"/>
+      <c r="B61" s="41"/>
       <c r="C61" s="26" t="s">
         <v>104</v>
       </c>
@@ -1869,7 +1872,7 @@
       </c>
     </row>
     <row r="62" spans="2:4">
-      <c r="B62" s="32"/>
+      <c r="B62" s="41"/>
       <c r="C62" s="26" t="s">
         <v>106</v>
       </c>
@@ -1878,7 +1881,7 @@
       </c>
     </row>
     <row r="63" spans="2:4">
-      <c r="B63" s="32"/>
+      <c r="B63" s="41"/>
       <c r="C63" s="26" t="s">
         <v>108</v>
       </c>
@@ -1887,7 +1890,7 @@
       </c>
     </row>
     <row r="64" spans="2:4">
-      <c r="B64" s="33"/>
+      <c r="B64" s="42"/>
       <c r="C64" s="23" t="s">
         <v>110</v>
       </c>
@@ -1896,7 +1899,7 @@
       </c>
     </row>
     <row r="65" spans="2:4">
-      <c r="B65" s="31" t="s">
+      <c r="B65" s="40" t="s">
         <v>30</v>
       </c>
       <c r="C65" s="18"/>
@@ -1905,7 +1908,7 @@
       </c>
     </row>
     <row r="66" spans="2:4">
-      <c r="B66" s="32"/>
+      <c r="B66" s="41"/>
       <c r="C66" s="26" t="s">
         <v>113</v>
       </c>
@@ -1914,7 +1917,7 @@
       </c>
     </row>
     <row r="67" spans="2:4">
-      <c r="B67" s="32"/>
+      <c r="B67" s="41"/>
       <c r="C67" s="26" t="s">
         <v>115</v>
       </c>
@@ -1923,7 +1926,7 @@
       </c>
     </row>
     <row r="68" spans="2:4">
-      <c r="B68" s="33"/>
+      <c r="B68" s="42"/>
       <c r="C68" s="23" t="s">
         <v>116</v>
       </c>
@@ -1941,11 +1944,11 @@
       </c>
     </row>
     <row r="71" spans="2:4">
-      <c r="B71" s="28" t="s">
+      <c r="B71" s="37" t="s">
         <v>119</v>
       </c>
-      <c r="C71" s="29"/>
-      <c r="D71" s="30"/>
+      <c r="C71" s="38"/>
+      <c r="D71" s="39"/>
     </row>
     <row r="72" spans="2:4">
       <c r="B72" s="15" t="s">
@@ -1959,7 +1962,7 @@
       </c>
     </row>
     <row r="73" spans="2:4">
-      <c r="B73" s="31" t="s">
+      <c r="B73" s="40" t="s">
         <v>99</v>
       </c>
       <c r="C73" s="18" t="s">
@@ -1970,7 +1973,7 @@
       </c>
     </row>
     <row r="74" spans="2:4">
-      <c r="B74" s="32"/>
+      <c r="B74" s="41"/>
       <c r="C74" s="12" t="s">
         <v>133</v>
       </c>
@@ -1979,7 +1982,7 @@
       </c>
     </row>
     <row r="75" spans="2:4">
-      <c r="B75" s="32"/>
+      <c r="B75" s="41"/>
       <c r="C75" s="12" t="s">
         <v>98</v>
       </c>
@@ -1988,7 +1991,7 @@
       </c>
     </row>
     <row r="76" spans="2:4">
-      <c r="B76" s="32"/>
+      <c r="B76" s="41"/>
       <c r="C76" s="12" t="s">
         <v>134</v>
       </c>
@@ -1997,7 +2000,7 @@
       </c>
     </row>
     <row r="77" spans="2:4">
-      <c r="B77" s="33"/>
+      <c r="B77" s="42"/>
       <c r="C77" s="14" t="s">
         <v>135</v>
       </c>
@@ -2006,7 +2009,7 @@
       </c>
     </row>
     <row r="78" spans="2:4">
-      <c r="B78" s="31" t="s">
+      <c r="B78" s="40" t="s">
         <v>129</v>
       </c>
       <c r="C78" s="18" t="s">
@@ -2017,7 +2020,7 @@
       </c>
     </row>
     <row r="79" spans="2:4">
-      <c r="B79" s="33"/>
+      <c r="B79" s="42"/>
       <c r="C79" s="14" t="s">
         <v>130</v>
       </c>
@@ -2046,7 +2049,7 @@
       </c>
     </row>
     <row r="82" spans="2:4">
-      <c r="B82" s="31" t="s">
+      <c r="B82" s="40" t="s">
         <v>121</v>
       </c>
       <c r="C82" s="18" t="s">
@@ -2057,7 +2060,7 @@
       </c>
     </row>
     <row r="83" spans="2:4">
-      <c r="B83" s="33"/>
+      <c r="B83" s="42"/>
       <c r="C83" s="14" t="s">
         <v>123</v>
       </c>
@@ -2066,7 +2069,7 @@
       </c>
     </row>
     <row r="84" spans="2:4">
-      <c r="B84" s="32" t="s">
+      <c r="B84" s="41" t="s">
         <v>30</v>
       </c>
       <c r="C84" s="12" t="s">
@@ -2077,14 +2080,14 @@
       </c>
     </row>
     <row r="85" spans="2:4">
-      <c r="B85" s="32"/>
+      <c r="B85" s="41"/>
       <c r="C85" s="12" t="s">
         <v>33</v>
       </c>
       <c r="D85" s="12"/>
     </row>
     <row r="86" spans="2:4">
-      <c r="B86" s="32"/>
+      <c r="B86" s="41"/>
       <c r="C86" s="12" t="s">
         <v>27</v>
       </c>
@@ -2093,7 +2096,7 @@
       </c>
     </row>
     <row r="87" spans="2:4">
-      <c r="B87" s="32"/>
+      <c r="B87" s="41"/>
       <c r="C87" s="12" t="s">
         <v>125</v>
       </c>
@@ -2102,7 +2105,7 @@
       </c>
     </row>
     <row r="88" spans="2:4">
-      <c r="B88" s="32"/>
+      <c r="B88" s="41"/>
       <c r="C88" s="12" t="s">
         <v>126</v>
       </c>
@@ -2111,7 +2114,7 @@
       </c>
     </row>
     <row r="89" spans="2:4">
-      <c r="B89" s="33"/>
+      <c r="B89" s="42"/>
       <c r="C89" s="14" t="s">
         <v>127</v>
       </c>
@@ -2125,267 +2128,264 @@
       <c r="D91" s="43"/>
     </row>
     <row r="92" spans="2:4">
-      <c r="B92" s="51" t="s">
+      <c r="B92" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C92" s="51" t="s">
+      <c r="C92" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D92" s="51" t="s">
+      <c r="D92" s="36" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="93" spans="2:4">
-      <c r="B93" s="32" t="s">
+      <c r="B93" s="41" t="s">
         <v>170</v>
       </c>
       <c r="C93" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="D93" s="44" t="s">
+      <c r="D93" s="29" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="94" spans="2:4" ht="30">
-      <c r="B94" s="32"/>
+      <c r="B94" s="41"/>
       <c r="C94" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="D94" s="45" t="s">
+      <c r="D94" s="30" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="95" spans="2:4" ht="30">
-      <c r="B95" s="32"/>
+      <c r="B95" s="41"/>
       <c r="C95" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="D95" s="45" t="s">
+      <c r="D95" s="30" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="96" spans="2:4">
-      <c r="B96" s="32"/>
+      <c r="B96" s="41"/>
       <c r="C96" s="26" t="s">
         <v>166</v>
       </c>
-      <c r="D96" s="46" t="s">
+      <c r="D96" s="31" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="97" spans="2:4">
-      <c r="B97" s="32"/>
+      <c r="B97" s="41"/>
       <c r="C97" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="D97" s="46" t="s">
+      <c r="D97" s="31" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="98" spans="2:4" ht="45">
-      <c r="B98" s="32"/>
+      <c r="B98" s="41"/>
       <c r="C98" s="26" t="s">
         <v>164</v>
       </c>
-      <c r="D98" s="45" t="s">
+      <c r="D98" s="30" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="99" spans="2:4">
-      <c r="B99" s="32"/>
+      <c r="B99" s="41"/>
       <c r="C99" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="D99" s="46" t="s">
+      <c r="D99" s="31" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="100" spans="2:4">
-      <c r="B100" s="32"/>
+      <c r="B100" s="41"/>
       <c r="C100" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="D100" s="46" t="s">
+      <c r="D100" s="31" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="101" spans="2:4">
-      <c r="B101" s="32"/>
+      <c r="B101" s="41"/>
       <c r="C101" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="D101" s="46" t="s">
+      <c r="D101" s="31" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="102" spans="2:4">
-      <c r="B102" s="32"/>
+      <c r="B102" s="41"/>
       <c r="C102" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="D102" s="46" t="s">
+      <c r="D102" s="31" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="103" spans="2:4">
-      <c r="B103" s="33"/>
+      <c r="B103" s="42"/>
       <c r="C103" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="D103" s="47" t="s">
+      <c r="D103" s="32" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="104" spans="2:4" ht="30">
-      <c r="B104" s="31" t="s">
+      <c r="B104" s="40" t="s">
         <v>156</v>
       </c>
-      <c r="C104" s="48" t="s">
+      <c r="C104" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="D104" s="49" t="s">
+      <c r="D104" s="34" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="105" spans="2:4">
-      <c r="B105" s="32"/>
+      <c r="B105" s="41"/>
       <c r="C105" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="D105" s="46" t="s">
+      <c r="D105" s="31" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="106" spans="2:4">
-      <c r="B106" s="32"/>
+      <c r="B106" s="41"/>
       <c r="C106" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="D106" s="46" t="s">
+      <c r="D106" s="31" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="107" spans="2:4">
-      <c r="B107" s="32"/>
+      <c r="B107" s="41"/>
       <c r="C107" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="D107" s="46"/>
+      <c r="D107" s="31"/>
     </row>
     <row r="108" spans="2:4">
-      <c r="B108" s="32"/>
+      <c r="B108" s="41"/>
       <c r="C108" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="D108" s="46" t="s">
+      <c r="D108" s="31" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="109" spans="2:4">
-      <c r="B109" s="32"/>
+      <c r="B109" s="41"/>
       <c r="C109" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="D109" s="46" t="s">
+      <c r="D109" s="31" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="110" spans="2:4">
-      <c r="B110" s="32"/>
+      <c r="B110" s="41"/>
       <c r="C110" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="D110" s="46" t="s">
+      <c r="D110" s="31" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="111" spans="2:4">
-      <c r="B111" s="32"/>
+      <c r="B111" s="41"/>
       <c r="C111" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="D111" s="46" t="s">
+      <c r="D111" s="31" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="112" spans="2:4" ht="45">
-      <c r="B112" s="32"/>
+      <c r="B112" s="41"/>
       <c r="C112" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D112" s="45" t="s">
+      <c r="D112" s="30" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="113" spans="2:4">
-      <c r="B113" s="33"/>
+      <c r="B113" s="42"/>
       <c r="C113" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="D113" s="50"/>
+      <c r="D113" s="35"/>
     </row>
     <row r="114" spans="2:4">
-      <c r="B114" s="32" t="s">
+      <c r="B114" s="41" t="s">
         <v>139</v>
       </c>
       <c r="C114" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="D114" s="46" t="s">
+      <c r="D114" s="31" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="115" spans="2:4">
-      <c r="B115" s="32"/>
+      <c r="B115" s="41"/>
       <c r="C115" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="D115" s="46"/>
+      <c r="D115" s="31"/>
     </row>
     <row r="116" spans="2:4">
-      <c r="B116" s="32"/>
+      <c r="B116" s="41"/>
       <c r="C116" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="D116" s="46" t="s">
+      <c r="D116" s="31" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="117" spans="2:4">
-      <c r="B117" s="32"/>
+      <c r="B117" s="41"/>
       <c r="C117" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="D117" s="46" t="s">
+      <c r="D117" s="31" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="118" spans="2:4">
-      <c r="B118" s="32"/>
+      <c r="B118" s="41"/>
       <c r="C118" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="D118" s="46"/>
+      <c r="D118" s="31"/>
     </row>
     <row r="119" spans="2:4">
-      <c r="B119" s="33"/>
+      <c r="B119" s="42"/>
       <c r="C119" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="D119" s="47" t="s">
+      <c r="D119" s="32" t="s">
         <v>138</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B104:B113"/>
-    <mergeCell ref="B114:B119"/>
-    <mergeCell ref="B91:D91"/>
-    <mergeCell ref="B93:B103"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="B59:B64"/>
-    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="B51:B53"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B71:D71"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B37:B40"/>
     <mergeCell ref="B17:B19"/>
@@ -2395,11 +2395,14 @@
     <mergeCell ref="B26:B31"/>
     <mergeCell ref="B20:B24"/>
     <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="B51:B53"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B104:B113"/>
+    <mergeCell ref="B114:B119"/>
+    <mergeCell ref="B91:D91"/>
+    <mergeCell ref="B93:B103"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B59:B64"/>
+    <mergeCell ref="B65:B68"/>
     <mergeCell ref="B73:B77"/>
     <mergeCell ref="B78:B79"/>
     <mergeCell ref="B82:B83"/>

</xml_diff>